<commit_message>
Fixed CDS sample testcase for study
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_CDS_Filter_Gender-Unknown.xlsx
+++ b/InputFiles/TC03_CDS_Filter_Gender-Unknown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Documents\Test_Automation_Copies\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27057FB-AB1C-4439-A69F-308BFEF37F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265A87C8-A373-4BED-987D-2569CE3ACE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -71,10 +71,40 @@
 WHERE p.gender in ["Unknown"]
 RETURN
     count(distinct s) AS Studies,
-    count(distinct diag.primary_diagnosis) AS `Disease Sites`,
     count(distinct p) AS Participants,
     count(distinct samp) AS Samples,
     count(distinct f) AS `Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+WHERE p.gender in ["Unknown"]
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT samp,diag,s,p
+RETURN  
+ coalesce(p.participant_id,'') as `Case ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(p.gender,'') as `Gender`,
+ coalesce(samp.sample_anatomic_site,'') as `Site`,
+ coalesce(samp.sample_id, '') as `Samples`
+ ORDER By p.participant_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+WHERE p.gender in ["Unknown"]
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH DISTINCT samp,diag,s,p
+RETURN  
+ coalesce(samp.sample_id, '') as `Sample ID` ,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(samp.sample_tumor_status,'') as `Tumor`,
+coalesce(samp.sample_type,'') as `Analyte Type`
+ORDER By samp.sample_id LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;--(p:participant)
@@ -90,52 +120,7 @@
     coalesce(p.participant_id,'') as `Subject ID`,
     coalesce(samp.sample_id, '') as `Sample ID`,
     coalesce(f.file_type, '') as `File Type`
-   ORDER By f.file_name</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE p.gender in ["Unknown"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p
-RETURN  
- coalesce(samp.sample_id, '') as `Sample ID` ,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(samp.sample_tumor_status,'') as `Tumor`,
-coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE p.gender in ["Unknown"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p
-RETURN  
- coalesce(p.participant_id,'') as `Case ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
- coalesce(samp.sample_anatomic_site,'') as `Site`,
- coalesce(samp.sample_id, '') as `Samples`
- ORDER By p.participant_id</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p,f
-WHERE  p.gender in ["Unknown"]
-RETURN
-    count(distinct s) AS Studies,
-    count(distinct diag.primary_diagnosis) AS `Disease Sites`,
-    count(distinct p) AS Participants,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Files`</t>
+   ORDER By f.file_name LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -518,7 +503,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -572,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -586,10 +571,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
merged CDS test suites to create CDS_Regression suite
</commit_message>
<xml_diff>
--- a/InputFiles/TC03_CDS_Filter_Gender-Unknown.xlsx
+++ b/InputFiles/TC03_CDS_Filter_Gender-Unknown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation 0707\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FA336B-F234-4FDB-A685-B055CD64CA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2609A-165D-4CB2-9CD6-7020C01C0E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -151,14 +151,14 @@
 WITH p
 OPTIONAL MATCH (p)--&gt;(s:study)
 OPTIONAL MATCH (samp:sample)--&gt;(p)
-WITH s, p, apoc.coll.sort(collect(distinct coalesce(samp.sample_id, "Not specified in data"))) as samp
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
 RETURN 
 coalesce(p.participant_id,'') as `Participant ID`,
 coalesce(s.study_name, '') as `Study Name`,
 coalesce(s.phs_accession,'') as `Accession`,
 coalesce(p.gender,'') as `Gender`,
 coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY p.participant_id LIMIT 100</t>
+ORDER BY p.participant_id limit 100</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>